<commit_message>
still too dumb to use directories ...
</commit_message>
<xml_diff>
--- a/FOE-Clicker/vikingTimes.xlsx
+++ b/FOE-Clicker/vikingTimes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stuff\FOE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stuff\FOE\clickerStuff\FOE-Clicker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF695B6-A1D8-4C3E-B5A3-3979009DBAA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4463D503-B061-45DA-AF50-0EF7B67A6ACC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{B514437C-18F7-4D4F-9A05-8D0CD7E47058}"/>
   </bookViews>
@@ -227,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -239,6 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -665,7 +666,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B7" sqref="B7:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,13 +710,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="D3" s="3">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="E3" s="3">
         <v>0</v>
@@ -735,52 +736,25 @@
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>22</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>37</v>
-      </c>
-      <c r="C7">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>83</v>
-      </c>
-      <c r="D8">
-        <v>22</v>
-      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
       <c r="E8"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>13</v>
-      </c>
-      <c r="C9">
-        <v>69</v>
-      </c>
-      <c r="D9">
-        <v>21</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -795,7 +769,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>11</v>
       </c>
@@ -812,7 +786,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>12</v>
       </c>
@@ -850,15 +824,15 @@
       </c>
       <c r="B14" s="1">
         <f>SUM(SUM(B4:B13),-B3)</f>
-        <v>128</v>
+        <v>13</v>
       </c>
       <c r="C14" s="1">
         <f>SUM(SUM(C4:C13),-C3)</f>
-        <v>398</v>
+        <v>98</v>
       </c>
       <c r="D14" s="1">
         <f>SUM(SUM(D4:D13),-D3)</f>
-        <v>142</v>
+        <v>43</v>
       </c>
       <c r="E14" s="1">
         <f>SUM(SUM(E4:E13),-E3)</f>
@@ -871,15 +845,15 @@
       </c>
       <c r="B15">
         <f>B14/5</f>
-        <v>25.6</v>
+        <v>2.6</v>
       </c>
       <c r="C15">
         <f>C14/5</f>
-        <v>79.599999999999994</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="D15">
         <f>D14/5</f>
-        <v>28.4</v>
+        <v>8.6</v>
       </c>
       <c r="E15">
         <f>E14/5</f>
@@ -892,15 +866,15 @@
       </c>
       <c r="B16">
         <f>B15*4/24</f>
-        <v>4.2666666666666666</v>
+        <v>0.43333333333333335</v>
       </c>
       <c r="C16">
         <f>C15*4/24</f>
-        <v>13.266666666666666</v>
+        <v>3.2666666666666671</v>
       </c>
       <c r="D16">
         <f>D15*4/24</f>
-        <v>4.7333333333333334</v>
+        <v>1.4333333333333333</v>
       </c>
       <c r="E16">
         <f>E15*4/24</f>
@@ -913,15 +887,15 @@
       </c>
       <c r="B17">
         <f>B16/B2</f>
-        <v>4.2666666666666666</v>
+        <v>0.43333333333333335</v>
       </c>
       <c r="C17">
         <f t="shared" ref="C17:E17" si="0">C16/C2</f>
-        <v>6.6333333333333329</v>
+        <v>1.6333333333333335</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>4.7333333333333334</v>
+        <v>1.4333333333333333</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>

</xml_diff>